<commit_message>
Eng Test Data - 12 Mar 2025
</commit_message>
<xml_diff>
--- a/TestData/T2263_CreateRevenueAccrual.xlsx
+++ b/TestData/T2263_CreateRevenueAccrual.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgoyal0427\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SGoyal0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF3AEBA-228C-4404-B7A3-F1A2394BDC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13155" windowHeight="2550" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -22,14 +23,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -61,9 +54,6 @@
     <t>BUS - Business Services</t>
   </si>
   <si>
-    <t>Dealership &amp; Rental Services</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -260,12 +250,15 @@
   </si>
   <si>
     <t>Chris Cessna</t>
+  </si>
+  <si>
+    <t>CSDN-0000001546</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -661,11 +654,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyFont="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -673,51 +664,54 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1 2" xfId="2"/>
-    <cellStyle name="20% - Accent2 2" xfId="7"/>
-    <cellStyle name="20% - Accent3 2" xfId="3"/>
-    <cellStyle name="20% - Accent4 2" xfId="4"/>
-    <cellStyle name="20% - Accent5 2" xfId="5"/>
-    <cellStyle name="20% - Accent6 2" xfId="6"/>
-    <cellStyle name="40% - Accent1 2" xfId="9"/>
-    <cellStyle name="40% - Accent2 2" xfId="7"/>
-    <cellStyle name="40% - Accent3 2" xfId="8"/>
-    <cellStyle name="40% - Accent4 2" xfId="10"/>
-    <cellStyle name="40% - Accent5 2" xfId="9"/>
-    <cellStyle name="40% - Accent6 2" xfId="10"/>
-    <cellStyle name="60% - Accent1 2" xfId="11"/>
-    <cellStyle name="60% - Accent2 2" xfId="12"/>
-    <cellStyle name="60% - Accent3 2" xfId="13"/>
-    <cellStyle name="60% - Accent4 2" xfId="14"/>
-    <cellStyle name="60% - Accent5 2" xfId="15"/>
-    <cellStyle name="60% - Accent6 2" xfId="20"/>
-    <cellStyle name="Accent1 2" xfId="15"/>
-    <cellStyle name="Accent2 2" xfId="16"/>
-    <cellStyle name="Accent3 2" xfId="17"/>
-    <cellStyle name="Accent4 2" xfId="18"/>
-    <cellStyle name="Accent5 2" xfId="19"/>
-    <cellStyle name="Accent6 2" xfId="20"/>
-    <cellStyle name="Bad 2" xfId="21"/>
-    <cellStyle name="Calculation 2" xfId="22"/>
-    <cellStyle name="Check Cell 2" xfId="23"/>
-    <cellStyle name="Explanatory Text 2" xfId="24"/>
-    <cellStyle name="Good 2" xfId="25"/>
-    <cellStyle name="Heading 1 2" xfId="26"/>
-    <cellStyle name="Heading 2 2" xfId="27"/>
-    <cellStyle name="Heading 3 2" xfId="28"/>
-    <cellStyle name="Heading 4 2" xfId="29"/>
-    <cellStyle name="Input 2" xfId="30"/>
-    <cellStyle name="Linked Cell 2" xfId="31"/>
-    <cellStyle name="Neutral 2" xfId="32"/>
+    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Calculation 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Check Cell 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="24" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Good 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Heading 1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Heading 2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Heading 3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Heading 4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Input 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Neutral 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Note 2" xfId="33"/>
-    <cellStyle name="Output 2" xfId="34"/>
-    <cellStyle name="Title 2" xfId="35"/>
-    <cellStyle name="Total 2" xfId="36"/>
-    <cellStyle name="Warning Text 2" xfId="37"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Note 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Output 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Title 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Total 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Warning Text 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -994,216 +988,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" style="3" customWidth="1"/>
-    <col min="15" max="17" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.85546875" style="3"/>
-    <col min="26" max="26" width="11.28515625" style="3" customWidth="1"/>
-    <col min="27" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.109375" customWidth="1"/>
+    <col min="15" max="17" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="V2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X2" t="s">
         <v>34</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Y2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>74</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1213,40 +1205,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1255,73 +1247,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1331,47 +1323,47 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>